<commit_message>
Added one new testcase Bill payment
</commit_message>
<xml_diff>
--- a/dataSheet/Test Data.xlsx
+++ b/dataSheet/Test Data.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>Testcase</t>
   </si>
@@ -101,6 +101,60 @@
   </si>
   <si>
     <t>Denied</t>
+  </si>
+  <si>
+    <t>TC005_BillPayment</t>
+  </si>
+  <si>
+    <t>Payee Name</t>
+  </si>
+  <si>
+    <t>ArunSekar</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Theni</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>9876</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>9080930255</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>5442589635</t>
+  </si>
+  <si>
+    <t>Verify Acc Number</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>850</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Kali Amman Kovil ST</t>
   </si>
 </sst>
 </file>
@@ -422,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -437,14 +491,16 @@
     <col min="5" max="5" width="20.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.21875" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.21875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="8" max="8" width="18.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.21875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.77734375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -466,7 +522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -500,7 +556,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:13">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -520,7 +576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -540,7 +596,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:13">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -563,7 +619,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -584,6 +640,89 @@
       </c>
       <c r="G11" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added assert in final screen pages alone
</commit_message>
<xml_diff>
--- a/dataSheet/Test Data.xlsx
+++ b/dataSheet/Test Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ParaBank_Selenium\dataSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ParaBank\dataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -100,9 +100,6 @@
     <t>13344</t>
   </si>
   <si>
-    <t>Denied</t>
-  </si>
-  <si>
     <t>TC005_BillPayment</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>Kali Amman Kovil ST</t>
+  </si>
+  <si>
+    <t>Submitted</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -639,7 +639,7 @@
         <v>21</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="H11" s="3"/>
     </row>
@@ -654,31 +654,31 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>11</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
@@ -695,31 +695,31 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>21</v>

</xml_diff>